<commit_message>
[EmailUtil.LeaveEmail] Update config and add images
</commit_message>
<xml_diff>
--- a/config/LeaveEmail.xlsx
+++ b/config/LeaveEmail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{A7445BA1-0B54-4F07-93B6-701A5B076C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73AD969C-0A45-4351-929A-CD927BE39F6D}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{A7445BA1-0B54-4F07-93B6-701A5B076C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F4D5DB-7BEC-472F-A046-4CEFE174FE06}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8A252A05-4B61-44C2-990E-D4DED5B9F39D}"/>
+    <workbookView xWindow="9648" yWindow="600" windowWidth="12072" windowHeight="11712" xr2:uid="{8A252A05-4B61-44C2-990E-D4DED5B9F39D}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +201,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -355,7 +361,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93D6FD10-21FB-466A-B951-9F2C7D59F846}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -391,7 +397,7 @@
                   <a:latin typeface="Arial"/>
                   <a:cs typeface="Arial"/>
                 </a:rPr>
-                <a:t>Gen for dates</a:t>
+                <a:t>Gen next in plan</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -722,7 +728,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>